<commit_message>
- (WIP) Report draft - Added DS2 NB validation output
</commit_message>
<xml_diff>
--- a/ds2/ds2_stats.xlsx
+++ b/ds2/ds2_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\Data set release 1\ds2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\soen472_mp2\ds2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78803629-5E8D-4950-86D0-B5E6A4CC1BF6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CCFE86-FBAF-47DC-9AE1-A900E25F64E1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" firstSheet="1" activeTab="2" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" xr2:uid="{E3F65C83-32B3-4C7A-966E-A0762FD703F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Training" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>Algorithm</t>
   </si>
@@ -158,12 +158,6 @@
     <t>Multilayer Perceptron (500 epochs / 10 hidden nodes)</t>
   </si>
   <si>
-    <t>Multilayer Perceptron (25 epochs / 517 hidden nodes)</t>
-  </si>
-  <si>
-    <t>Using same hyper-parameters as training</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -204,6 +198,21 @@
   </si>
   <si>
     <t>Same tree, same metrics, higher error rate</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Using same hyper-parameters as training. Note that DS2 is unbalanced.</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Class 6 (lambda) is all FN. Precision and F-measure could not be calculated.</t>
+  </si>
+  <si>
+    <t>Multilayer Perceptron (10 epochs / 517 hidden nodes)</t>
   </si>
 </sst>
 </file>
@@ -275,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -288,6 +297,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,19 +615,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C695380-AF5B-45A7-BF2D-28CA00309EBE}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" style="1" customWidth="1"/>
     <col min="2" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,8 +644,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -649,7 +665,7 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -666,7 +682,7 @@
         <v>0.94499999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -683,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,12 +716,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
@@ -730,19 +761,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E241F916-2D09-489E-8D95-B541D8A8FAFC}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" customWidth="1"/>
     <col min="2" max="5" width="13.6328125" customWidth="1"/>
+    <col min="6" max="6" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,8 +790,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -776,7 +811,7 @@
         <v>0.80300000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -793,22 +828,37 @@
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>40</v>
       </c>
@@ -825,9 +875,9 @@
         <v>0.85499999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -846,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DCDAD8C-75AB-4CEE-AB9A-0DE9B2745C0F}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -864,10 +914,10 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -875,7 +925,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -886,7 +936,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -897,7 +947,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -908,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -919,7 +969,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -930,10 +980,10 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>0.25</v>
@@ -944,7 +994,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -955,7 +1005,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -966,10 +1016,10 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -980,10 +1030,10 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -994,10 +1044,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1008,10 +1058,10 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1022,7 +1072,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1033,10 +1083,10 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1047,7 +1097,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1058,7 +1108,7 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>

</xml_diff>